<commit_message>
Added handler of yt stream , TODO rest of code...
</commit_message>
<xml_diff>
--- a/results1.xlsx
+++ b/results1.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D134"/>
+  <dimension ref="A1:D229"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2837,6 +2837,1716 @@
         </is>
       </c>
     </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:24:25</t>
+        </is>
+      </c>
+      <c r="B135" t="n">
+        <v>0</v>
+      </c>
+      <c r="C135" t="n">
+        <v>0</v>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>0.10 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:24:26</t>
+        </is>
+      </c>
+      <c r="B136" t="n">
+        <v>0</v>
+      </c>
+      <c r="C136" t="n">
+        <v>0</v>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>0.21 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:24:27</t>
+        </is>
+      </c>
+      <c r="B137" t="n">
+        <v>0</v>
+      </c>
+      <c r="C137" t="n">
+        <v>0</v>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>0.31 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:24:28</t>
+        </is>
+      </c>
+      <c r="B138" t="n">
+        <v>0</v>
+      </c>
+      <c r="C138" t="n">
+        <v>0</v>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>0.41 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:24:29</t>
+        </is>
+      </c>
+      <c r="B139" t="n">
+        <v>0</v>
+      </c>
+      <c r="C139" t="n">
+        <v>0</v>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>0.52 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:24:30</t>
+        </is>
+      </c>
+      <c r="B140" t="n">
+        <v>0</v>
+      </c>
+      <c r="C140" t="n">
+        <v>0</v>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>0.62 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:24:31</t>
+        </is>
+      </c>
+      <c r="B141" t="n">
+        <v>0</v>
+      </c>
+      <c r="C141" t="n">
+        <v>0</v>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>0.72 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:24:32</t>
+        </is>
+      </c>
+      <c r="B142" t="n">
+        <v>0</v>
+      </c>
+      <c r="C142" t="n">
+        <v>0</v>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>0.83 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:24:32</t>
+        </is>
+      </c>
+      <c r="B143" t="n">
+        <v>0</v>
+      </c>
+      <c r="C143" t="n">
+        <v>0</v>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>0.93 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:24:34</t>
+        </is>
+      </c>
+      <c r="B144" t="n">
+        <v>0</v>
+      </c>
+      <c r="C144" t="n">
+        <v>0</v>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>1.03 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:24:34</t>
+        </is>
+      </c>
+      <c r="B145" t="n">
+        <v>0</v>
+      </c>
+      <c r="C145" t="n">
+        <v>0</v>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>1.14 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:24:35</t>
+        </is>
+      </c>
+      <c r="B146" t="n">
+        <v>0</v>
+      </c>
+      <c r="C146" t="n">
+        <v>0</v>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>1.24 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:24:36</t>
+        </is>
+      </c>
+      <c r="B147" t="n">
+        <v>0</v>
+      </c>
+      <c r="C147" t="n">
+        <v>0</v>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>1.34 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:24:37</t>
+        </is>
+      </c>
+      <c r="B148" t="n">
+        <v>0</v>
+      </c>
+      <c r="C148" t="n">
+        <v>0</v>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>1.45 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:24:38</t>
+        </is>
+      </c>
+      <c r="B149" t="n">
+        <v>0</v>
+      </c>
+      <c r="C149" t="n">
+        <v>0</v>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>1.55 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:24:39</t>
+        </is>
+      </c>
+      <c r="B150" t="n">
+        <v>0</v>
+      </c>
+      <c r="C150" t="n">
+        <v>0</v>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>1.66 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:24:40</t>
+        </is>
+      </c>
+      <c r="B151" t="n">
+        <v>0</v>
+      </c>
+      <c r="C151" t="n">
+        <v>0</v>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>1.76 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:24:41</t>
+        </is>
+      </c>
+      <c r="B152" t="n">
+        <v>0</v>
+      </c>
+      <c r="C152" t="n">
+        <v>0</v>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>1.86 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:24:42</t>
+        </is>
+      </c>
+      <c r="B153" t="n">
+        <v>0</v>
+      </c>
+      <c r="C153" t="n">
+        <v>0</v>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>1.97 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:24:43</t>
+        </is>
+      </c>
+      <c r="B154" t="n">
+        <v>0</v>
+      </c>
+      <c r="C154" t="n">
+        <v>0</v>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>2.07 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:24:44</t>
+        </is>
+      </c>
+      <c r="B155" t="n">
+        <v>0</v>
+      </c>
+      <c r="C155" t="n">
+        <v>0</v>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>2.17 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:24:45</t>
+        </is>
+      </c>
+      <c r="B156" t="n">
+        <v>0</v>
+      </c>
+      <c r="C156" t="n">
+        <v>0</v>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>2.28 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:24:46</t>
+        </is>
+      </c>
+      <c r="B157" t="n">
+        <v>0</v>
+      </c>
+      <c r="C157" t="n">
+        <v>0</v>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>2.38 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:24:47</t>
+        </is>
+      </c>
+      <c r="B158" t="n">
+        <v>0</v>
+      </c>
+      <c r="C158" t="n">
+        <v>0</v>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>2.48 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:24:48</t>
+        </is>
+      </c>
+      <c r="B159" t="n">
+        <v>0</v>
+      </c>
+      <c r="C159" t="n">
+        <v>0</v>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>2.59 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:24:49</t>
+        </is>
+      </c>
+      <c r="B160" t="n">
+        <v>0</v>
+      </c>
+      <c r="C160" t="n">
+        <v>0</v>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>2.69 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:24:50</t>
+        </is>
+      </c>
+      <c r="B161" t="n">
+        <v>0</v>
+      </c>
+      <c r="C161" t="n">
+        <v>0</v>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>2.79 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:24:51</t>
+        </is>
+      </c>
+      <c r="B162" t="n">
+        <v>0</v>
+      </c>
+      <c r="C162" t="n">
+        <v>0</v>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>2.90 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:24:52</t>
+        </is>
+      </c>
+      <c r="B163" t="n">
+        <v>0</v>
+      </c>
+      <c r="C163" t="n">
+        <v>0</v>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>3.00 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:24:53</t>
+        </is>
+      </c>
+      <c r="B164" t="n">
+        <v>0</v>
+      </c>
+      <c r="C164" t="n">
+        <v>0</v>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>3.10 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:24:54</t>
+        </is>
+      </c>
+      <c r="B165" t="n">
+        <v>0</v>
+      </c>
+      <c r="C165" t="n">
+        <v>0</v>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>3.21 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:24:55</t>
+        </is>
+      </c>
+      <c r="B166" t="n">
+        <v>0</v>
+      </c>
+      <c r="C166" t="n">
+        <v>0</v>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>3.31 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:24:56</t>
+        </is>
+      </c>
+      <c r="B167" t="n">
+        <v>0</v>
+      </c>
+      <c r="C167" t="n">
+        <v>0</v>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>3.41 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:24:57</t>
+        </is>
+      </c>
+      <c r="B168" t="n">
+        <v>0</v>
+      </c>
+      <c r="C168" t="n">
+        <v>0</v>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>3.52 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:24:58</t>
+        </is>
+      </c>
+      <c r="B169" t="n">
+        <v>0</v>
+      </c>
+      <c r="C169" t="n">
+        <v>0</v>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>3.62 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:24:59</t>
+        </is>
+      </c>
+      <c r="B170" t="n">
+        <v>0</v>
+      </c>
+      <c r="C170" t="n">
+        <v>0</v>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>3.72 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:25:00</t>
+        </is>
+      </c>
+      <c r="B171" t="n">
+        <v>0</v>
+      </c>
+      <c r="C171" t="n">
+        <v>0</v>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>3.83 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:25:01</t>
+        </is>
+      </c>
+      <c r="B172" t="n">
+        <v>0</v>
+      </c>
+      <c r="C172" t="n">
+        <v>0</v>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>3.93 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:25:02</t>
+        </is>
+      </c>
+      <c r="B173" t="n">
+        <v>0</v>
+      </c>
+      <c r="C173" t="n">
+        <v>0</v>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>4.03 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:25:03</t>
+        </is>
+      </c>
+      <c r="B174" t="n">
+        <v>0</v>
+      </c>
+      <c r="C174" t="n">
+        <v>0</v>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>4.14 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:25:04</t>
+        </is>
+      </c>
+      <c r="B175" t="n">
+        <v>0</v>
+      </c>
+      <c r="C175" t="n">
+        <v>0</v>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>4.24 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:25:05</t>
+        </is>
+      </c>
+      <c r="B176" t="n">
+        <v>0</v>
+      </c>
+      <c r="C176" t="n">
+        <v>0</v>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>4.34 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:25:06</t>
+        </is>
+      </c>
+      <c r="B177" t="n">
+        <v>0</v>
+      </c>
+      <c r="C177" t="n">
+        <v>0</v>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>4.45 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:38:39</t>
+        </is>
+      </c>
+      <c r="B178" t="n">
+        <v>0</v>
+      </c>
+      <c r="C178" t="n">
+        <v>0</v>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>0.10 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:38:40</t>
+        </is>
+      </c>
+      <c r="B179" t="n">
+        <v>0</v>
+      </c>
+      <c r="C179" t="n">
+        <v>0</v>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>0.21 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:38:41</t>
+        </is>
+      </c>
+      <c r="B180" t="n">
+        <v>0</v>
+      </c>
+      <c r="C180" t="n">
+        <v>0</v>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>0.31 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:38:42</t>
+        </is>
+      </c>
+      <c r="B181" t="n">
+        <v>0</v>
+      </c>
+      <c r="C181" t="n">
+        <v>0</v>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>0.41 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:38:43</t>
+        </is>
+      </c>
+      <c r="B182" t="n">
+        <v>0</v>
+      </c>
+      <c r="C182" t="n">
+        <v>0</v>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>0.52 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:38:44</t>
+        </is>
+      </c>
+      <c r="B183" t="n">
+        <v>0</v>
+      </c>
+      <c r="C183" t="n">
+        <v>0</v>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>0.62 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:38:45</t>
+        </is>
+      </c>
+      <c r="B184" t="n">
+        <v>0</v>
+      </c>
+      <c r="C184" t="n">
+        <v>0</v>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>0.72 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:38:46</t>
+        </is>
+      </c>
+      <c r="B185" t="n">
+        <v>0</v>
+      </c>
+      <c r="C185" t="n">
+        <v>0</v>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>0.83 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:38:47</t>
+        </is>
+      </c>
+      <c r="B186" t="n">
+        <v>0</v>
+      </c>
+      <c r="C186" t="n">
+        <v>0</v>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>0.93 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:38:48</t>
+        </is>
+      </c>
+      <c r="B187" t="n">
+        <v>0</v>
+      </c>
+      <c r="C187" t="n">
+        <v>0</v>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>1.03 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:38:49</t>
+        </is>
+      </c>
+      <c r="B188" t="n">
+        <v>0</v>
+      </c>
+      <c r="C188" t="n">
+        <v>0</v>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>1.14 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:38:50</t>
+        </is>
+      </c>
+      <c r="B189" t="n">
+        <v>0</v>
+      </c>
+      <c r="C189" t="n">
+        <v>0</v>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>1.24 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:38:51</t>
+        </is>
+      </c>
+      <c r="B190" t="n">
+        <v>0</v>
+      </c>
+      <c r="C190" t="n">
+        <v>0</v>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>1.34 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:38:52</t>
+        </is>
+      </c>
+      <c r="B191" t="n">
+        <v>0</v>
+      </c>
+      <c r="C191" t="n">
+        <v>0</v>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>1.45 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:38:53</t>
+        </is>
+      </c>
+      <c r="B192" t="n">
+        <v>0</v>
+      </c>
+      <c r="C192" t="n">
+        <v>0</v>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>1.55 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:38:54</t>
+        </is>
+      </c>
+      <c r="B193" t="n">
+        <v>0</v>
+      </c>
+      <c r="C193" t="n">
+        <v>0</v>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>1.66 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:38:55</t>
+        </is>
+      </c>
+      <c r="B194" t="n">
+        <v>0</v>
+      </c>
+      <c r="C194" t="n">
+        <v>0</v>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>1.76 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:38:56</t>
+        </is>
+      </c>
+      <c r="B195" t="n">
+        <v>0</v>
+      </c>
+      <c r="C195" t="n">
+        <v>0</v>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>1.86 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:38:57</t>
+        </is>
+      </c>
+      <c r="B196" t="n">
+        <v>0</v>
+      </c>
+      <c r="C196" t="n">
+        <v>0</v>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>1.97 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:38:58</t>
+        </is>
+      </c>
+      <c r="B197" t="n">
+        <v>0</v>
+      </c>
+      <c r="C197" t="n">
+        <v>0</v>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>2.07 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:38:59</t>
+        </is>
+      </c>
+      <c r="B198" t="n">
+        <v>0</v>
+      </c>
+      <c r="C198" t="n">
+        <v>0</v>
+      </c>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>2.17 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:39:00</t>
+        </is>
+      </c>
+      <c r="B199" t="n">
+        <v>0</v>
+      </c>
+      <c r="C199" t="n">
+        <v>0</v>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>2.28 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:39:01</t>
+        </is>
+      </c>
+      <c r="B200" t="n">
+        <v>0</v>
+      </c>
+      <c r="C200" t="n">
+        <v>0</v>
+      </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>2.38 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:39:02</t>
+        </is>
+      </c>
+      <c r="B201" t="n">
+        <v>0</v>
+      </c>
+      <c r="C201" t="n">
+        <v>0</v>
+      </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>2.48 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:39:03</t>
+        </is>
+      </c>
+      <c r="B202" t="n">
+        <v>0</v>
+      </c>
+      <c r="C202" t="n">
+        <v>0</v>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>2.59 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:39:03</t>
+        </is>
+      </c>
+      <c r="B203" t="n">
+        <v>0</v>
+      </c>
+      <c r="C203" t="n">
+        <v>0</v>
+      </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>2.69 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:39:04</t>
+        </is>
+      </c>
+      <c r="B204" t="n">
+        <v>0</v>
+      </c>
+      <c r="C204" t="n">
+        <v>0</v>
+      </c>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>2.79 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:39:05</t>
+        </is>
+      </c>
+      <c r="B205" t="n">
+        <v>0</v>
+      </c>
+      <c r="C205" t="n">
+        <v>0</v>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>2.90 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:39:06</t>
+        </is>
+      </c>
+      <c r="B206" t="n">
+        <v>0</v>
+      </c>
+      <c r="C206" t="n">
+        <v>0</v>
+      </c>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>3.00 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:39:07</t>
+        </is>
+      </c>
+      <c r="B207" t="n">
+        <v>0</v>
+      </c>
+      <c r="C207" t="n">
+        <v>0</v>
+      </c>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>3.10 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:39:08</t>
+        </is>
+      </c>
+      <c r="B208" t="n">
+        <v>0</v>
+      </c>
+      <c r="C208" t="n">
+        <v>0</v>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>3.21 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:39:09</t>
+        </is>
+      </c>
+      <c r="B209" t="n">
+        <v>0</v>
+      </c>
+      <c r="C209" t="n">
+        <v>0</v>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>3.31 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:39:10</t>
+        </is>
+      </c>
+      <c r="B210" t="n">
+        <v>0</v>
+      </c>
+      <c r="C210" t="n">
+        <v>0</v>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>3.41 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:39:11</t>
+        </is>
+      </c>
+      <c r="B211" t="n">
+        <v>0</v>
+      </c>
+      <c r="C211" t="n">
+        <v>0</v>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>3.52 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:39:12</t>
+        </is>
+      </c>
+      <c r="B212" t="n">
+        <v>0</v>
+      </c>
+      <c r="C212" t="n">
+        <v>0</v>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>3.62 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:39:13</t>
+        </is>
+      </c>
+      <c r="B213" t="n">
+        <v>0</v>
+      </c>
+      <c r="C213" t="n">
+        <v>0</v>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>3.72 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:39:14</t>
+        </is>
+      </c>
+      <c r="B214" t="n">
+        <v>0</v>
+      </c>
+      <c r="C214" t="n">
+        <v>0</v>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>3.83 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:39:15</t>
+        </is>
+      </c>
+      <c r="B215" t="n">
+        <v>0</v>
+      </c>
+      <c r="C215" t="n">
+        <v>0</v>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>3.93 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:39:16</t>
+        </is>
+      </c>
+      <c r="B216" t="n">
+        <v>0</v>
+      </c>
+      <c r="C216" t="n">
+        <v>0</v>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>4.03 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:39:17</t>
+        </is>
+      </c>
+      <c r="B217" t="n">
+        <v>0</v>
+      </c>
+      <c r="C217" t="n">
+        <v>0</v>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>4.14 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:39:18</t>
+        </is>
+      </c>
+      <c r="B218" t="n">
+        <v>0</v>
+      </c>
+      <c r="C218" t="n">
+        <v>0</v>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>4.24 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:39:19</t>
+        </is>
+      </c>
+      <c r="B219" t="n">
+        <v>0</v>
+      </c>
+      <c r="C219" t="n">
+        <v>0</v>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>4.34 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:39:20</t>
+        </is>
+      </c>
+      <c r="B220" t="n">
+        <v>0</v>
+      </c>
+      <c r="C220" t="n">
+        <v>0</v>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>4.45 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:39:21</t>
+        </is>
+      </c>
+      <c r="B221" t="n">
+        <v>0</v>
+      </c>
+      <c r="C221" t="n">
+        <v>0</v>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>4.55 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:39:22</t>
+        </is>
+      </c>
+      <c r="B222" t="n">
+        <v>0</v>
+      </c>
+      <c r="C222" t="n">
+        <v>0</v>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>4.66 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:39:23</t>
+        </is>
+      </c>
+      <c r="B223" t="n">
+        <v>0</v>
+      </c>
+      <c r="C223" t="n">
+        <v>0</v>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>4.76 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:39:24</t>
+        </is>
+      </c>
+      <c r="B224" t="n">
+        <v>0</v>
+      </c>
+      <c r="C224" t="n">
+        <v>0</v>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>4.86 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:39:25</t>
+        </is>
+      </c>
+      <c r="B225" t="n">
+        <v>0</v>
+      </c>
+      <c r="C225" t="n">
+        <v>0</v>
+      </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>4.97 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:39:26</t>
+        </is>
+      </c>
+      <c r="B226" t="n">
+        <v>0</v>
+      </c>
+      <c r="C226" t="n">
+        <v>0</v>
+      </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>5.07 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:39:27</t>
+        </is>
+      </c>
+      <c r="B227" t="n">
+        <v>0</v>
+      </c>
+      <c r="C227" t="n">
+        <v>0</v>
+      </c>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>5.17 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:39:28</t>
+        </is>
+      </c>
+      <c r="B228" t="n">
+        <v>0</v>
+      </c>
+      <c r="C228" t="n">
+        <v>0</v>
+      </c>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>5.28 seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>2024-05-08 15:39:30</t>
+        </is>
+      </c>
+      <c r="B229" t="n">
+        <v>0</v>
+      </c>
+      <c r="C229" t="n">
+        <v>0</v>
+      </c>
+      <c r="D229" t="inlineStr">
+        <is>
+          <t>5.38 seconds</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>